<commit_message>
Added New Tables for Diagonisis,Allergies
</commit_message>
<xml_diff>
--- a/PMS-DB-Tables.xlsx
+++ b/PMS-DB-Tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GauravO\Documents\Training-Docs\Impact Training\Project\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87B938-F95A-4BB0-963F-36C339B72DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADEB917-7BE2-4653-8819-25C92E4014A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A88FE164-5C32-4E6C-9A73-9294D92DE1E9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A88FE164-5C32-4E6C-9A73-9294D92DE1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="User Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Master-Data Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>User Table</t>
   </si>
@@ -97,19 +98,322 @@
   </si>
   <si>
     <t>PrimaryKey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DrugData </t>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_ID –(Snomed-ct)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_Name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_Generic_Name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>d.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_Brand_Name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_Form – (Oral, Injection, Tablet, Powder, Cream, Capsule, Solution, Ointment, Syrup etc.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Drug_Strength – (5MG/ML, 20,000 UNITS/ML, 15MG, 12GM/50ML, 5ML/100ML etc.)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosis </t>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diagnosis_Code (A00, A00.1, B00)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diagnosis_Description (Cholera, Cholera due to Vibrio cholerae 01, biovar cholerae, Typhoid etc)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diagnosis_Is_Depricated (Boolean)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Procedure </t>
+  </si>
+  <si>
+    <r>
+      <t>a.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Procedure_Code (001607A)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>b.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Procedure_Description (Bypass Cerebral Ventricle to Subgaleal Space with Autologous Tissue Substitute, Open Approach)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>c.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Procedure_Is_Depricated (Boolean)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,9 +442,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="14"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51286AB1-6015-499B-B329-1E14C7DE5141}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -576,4 +883,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB788C50-9836-40BD-9197-B7FC0A3259CD}">
+  <dimension ref="A2:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>